<commit_message>
Comments added to DistanceMatrix.xlsx
</commit_message>
<xml_diff>
--- a/Data/DistanceMatrix.xlsx
+++ b/Data/DistanceMatrix.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7FAE048-3AB3-47E7-9BB7-7486320AE62E}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B6827D-8E27-4FC1-8865-F9341DA3A9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix 50x50" sheetId="2" r:id="rId1"/>
@@ -25,15 +30,110 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>-</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2632D36C-438D-4DA9-9B02-D1B73B9AE49E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>-:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Distance from point 0 to point 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{5794B927-50C5-42DD-9B17-3BC86D27D51C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>-:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Distance from point 2 to point 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{B5387C3F-6934-4447-81D4-2101CA30ABCB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>-:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Distance from point 2 to point 3</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -371,14 +471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15887770-4BB0-4391-9A36-27D1B5FA0955}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15887770-4BB0-4391-9A36-27D1B5FA0955}">
   <dimension ref="A1:AX50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -530,7 +630,7 @@
         <v>62.15</v>
       </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>51.79</v>
       </c>
@@ -682,7 +782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:50">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13.08</v>
       </c>
@@ -834,7 +934,7 @@
         <v>13.27</v>
       </c>
     </row>
-    <row r="4" spans="1:50">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>42.03</v>
       </c>
@@ -986,7 +1086,7 @@
         <v>21.24</v>
       </c>
     </row>
-    <row r="5" spans="1:50">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>76.78</v>
       </c>
@@ -1138,7 +1238,7 @@
         <v>30.15</v>
       </c>
     </row>
-    <row r="6" spans="1:50">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>73.16</v>
       </c>
@@ -1290,7 +1390,7 @@
         <v>54.18</v>
       </c>
     </row>
-    <row r="7" spans="1:50">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>36.06</v>
       </c>
@@ -1442,7 +1542,7 @@
         <v>11.32</v>
       </c>
     </row>
-    <row r="8" spans="1:50">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>18.75</v>
       </c>
@@ -1594,7 +1694,7 @@
         <v>20.34</v>
       </c>
     </row>
-    <row r="9" spans="1:50">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9.42</v>
       </c>
@@ -1746,7 +1846,7 @@
         <v>59.8</v>
       </c>
     </row>
-    <row r="10" spans="1:50">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>38.630000000000003</v>
       </c>
@@ -1898,7 +1998,7 @@
         <v>73.91</v>
       </c>
     </row>
-    <row r="11" spans="1:50">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>77.400000000000006</v>
       </c>
@@ -2050,7 +2150,7 @@
         <v>52.23</v>
       </c>
     </row>
-    <row r="12" spans="1:50">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>74.66</v>
       </c>
@@ -2202,7 +2302,7 @@
         <v>23.76</v>
       </c>
     </row>
-    <row r="13" spans="1:50">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43.46</v>
       </c>
@@ -2354,7 +2454,7 @@
         <v>92.63</v>
       </c>
     </row>
-    <row r="14" spans="1:50">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>18.37</v>
       </c>
@@ -2506,7 +2606,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="15" spans="1:50">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10.9</v>
       </c>
@@ -2658,7 +2758,7 @@
         <v>51.48</v>
       </c>
     </row>
-    <row r="16" spans="1:50">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50.63</v>
       </c>
@@ -2810,7 +2910,7 @@
         <v>87.07</v>
       </c>
     </row>
-    <row r="17" spans="1:50">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60.36</v>
       </c>
@@ -2962,7 +3062,7 @@
         <v>92.13</v>
       </c>
     </row>
-    <row r="18" spans="1:50">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>76.44</v>
       </c>
@@ -3114,7 +3214,7 @@
         <v>88.74</v>
       </c>
     </row>
-    <row r="19" spans="1:50">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>49.51</v>
       </c>
@@ -3266,7 +3366,7 @@
         <v>28.86</v>
       </c>
     </row>
-    <row r="20" spans="1:50">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14.98</v>
       </c>
@@ -3418,7 +3518,7 @@
         <v>94.51</v>
       </c>
     </row>
-    <row r="21" spans="1:50">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>99.71</v>
       </c>
@@ -3570,7 +3670,7 @@
         <v>55.02</v>
       </c>
     </row>
-    <row r="22" spans="1:50">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>58.22</v>
       </c>
@@ -3722,7 +3822,7 @@
         <v>50.59</v>
       </c>
     </row>
-    <row r="23" spans="1:50">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>83.45</v>
       </c>
@@ -3874,7 +3974,7 @@
         <v>93.29</v>
       </c>
     </row>
-    <row r="24" spans="1:50">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>49.47</v>
       </c>
@@ -4026,7 +4126,7 @@
         <v>73.75</v>
       </c>
     </row>
-    <row r="25" spans="1:50">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>75.27</v>
       </c>
@@ -4178,7 +4278,7 @@
         <v>85.91</v>
       </c>
     </row>
-    <row r="26" spans="1:50">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>32.03</v>
       </c>
@@ -4330,7 +4430,7 @@
         <v>75.680000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:50">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>68.760000000000005</v>
       </c>
@@ -4482,7 +4582,7 @@
         <v>75.94</v>
       </c>
     </row>
-    <row r="28" spans="1:50">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>41.81</v>
       </c>
@@ -4634,7 +4734,7 @@
         <v>85.52</v>
       </c>
     </row>
-    <row r="29" spans="1:50">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20.75</v>
       </c>
@@ -4786,7 +4886,7 @@
         <v>53.9</v>
       </c>
     </row>
-    <row r="30" spans="1:50">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>78.53</v>
       </c>
@@ -4938,7 +5038,7 @@
         <v>52.33</v>
       </c>
     </row>
-    <row r="31" spans="1:50">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>73.19</v>
       </c>
@@ -5090,7 +5190,7 @@
         <v>55.32</v>
       </c>
     </row>
-    <row r="32" spans="1:50">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>81.93</v>
       </c>
@@ -5242,7 +5342,7 @@
         <v>63.76</v>
       </c>
     </row>
-    <row r="33" spans="1:50">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>58.05</v>
       </c>
@@ -5394,7 +5494,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="34" spans="1:50">
+    <row r="34" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>98.74</v>
       </c>
@@ -5546,7 +5646,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="35" spans="1:50">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>80.55</v>
       </c>
@@ -5698,7 +5798,7 @@
         <v>79.37</v>
       </c>
     </row>
-    <row r="36" spans="1:50">
+    <row r="36" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>37.72</v>
       </c>
@@ -5850,7 +5950,7 @@
         <v>16.14</v>
       </c>
     </row>
-    <row r="37" spans="1:50">
+    <row r="37" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>63.31</v>
       </c>
@@ -6002,7 +6102,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="38" spans="1:50">
+    <row r="38" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>53.46</v>
       </c>
@@ -6154,7 +6254,7 @@
         <v>75.73</v>
       </c>
     </row>
-    <row r="39" spans="1:50">
+    <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>58.64</v>
       </c>
@@ -6306,7 +6406,7 @@
         <v>72.11</v>
       </c>
     </row>
-    <row r="40" spans="1:50">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>23.7</v>
       </c>
@@ -6458,7 +6558,7 @@
         <v>58.13</v>
       </c>
     </row>
-    <row r="41" spans="1:50">
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>51.57</v>
       </c>
@@ -6610,7 +6710,7 @@
         <v>98.04</v>
       </c>
     </row>
-    <row r="42" spans="1:50">
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>82.81</v>
       </c>
@@ -6762,7 +6862,7 @@
         <v>4.93</v>
       </c>
     </row>
-    <row r="43" spans="1:50">
+    <row r="43" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>66.13</v>
       </c>
@@ -6914,7 +7014,7 @@
         <v>62.35</v>
       </c>
     </row>
-    <row r="44" spans="1:50">
+    <row r="44" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>70.349999999999994</v>
       </c>
@@ -7066,7 +7166,7 @@
         <v>82.63</v>
       </c>
     </row>
-    <row r="45" spans="1:50">
+    <row r="45" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>47.1</v>
       </c>
@@ -7218,7 +7318,7 @@
         <v>83.97</v>
       </c>
     </row>
-    <row r="46" spans="1:50">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>32.65</v>
       </c>
@@ -7370,7 +7470,7 @@
         <v>45.14</v>
       </c>
     </row>
-    <row r="47" spans="1:50">
+    <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60.3</v>
       </c>
@@ -7522,7 +7622,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="48" spans="1:50">
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>97.04</v>
       </c>
@@ -7674,7 +7774,7 @@
         <v>60.76</v>
       </c>
     </row>
-    <row r="49" spans="1:50">
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>77.180000000000007</v>
       </c>
@@ -7826,7 +7926,7 @@
         <v>18.73</v>
       </c>
     </row>
-    <row r="50" spans="1:50">
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>86.57</v>
       </c>
@@ -7980,5 +8080,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>